<commit_message>
upload all experiments and update progress
</commit_message>
<xml_diff>
--- a/Formal_Exp.xlsx
+++ b/Formal_Exp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yunlong\Desktop\Recommender-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F75690C-B8E7-4E09-BDF2-121F09CB0C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1938E8F-494C-40D7-A361-72E1E9AF8277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52695" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43200" yWindow="1200" windowWidth="21600" windowHeight="12525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="42">
   <si>
     <t>dataset</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -174,9 +174,6 @@
   <si>
     <t>ml-20m</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Transfer learning</t>
   </si>
   <si>
     <t>t2v_normal_sasrec</t>
@@ -211,7 +208,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,19 +221,6 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -278,13 +262,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -567,9 +549,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J56" sqref="J56"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -638,7 +620,7 @@
         <v>18</v>
       </c>
       <c r="S1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:30">
@@ -951,11 +933,11 @@
         <v>24</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G12" si="4">AVERAGE(I7,K7,M7,O7,Q7)</f>
+        <f t="shared" ref="G7:G10" si="4">AVERAGE(I7,K7,M7,O7,Q7)</f>
         <v>0.44874000000000003</v>
       </c>
       <c r="H7">
-        <f t="shared" ref="H7:H12" si="5">AVERAGE(J7,L7,N7,P7,R7)</f>
+        <f t="shared" ref="H7:H10" si="5">AVERAGE(J7,L7,N7,P7,R7)</f>
         <v>0.27086000000000005</v>
       </c>
       <c r="I7">
@@ -1164,30 +1146,30 @@
       </c>
     </row>
     <row r="11" spans="1:30">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:G15" si="6">AVERAGE(I11,K11,M11,O11,Q11)</f>
+        <f t="shared" ref="G11:G12" si="6">AVERAGE(I11,K11,M11,O11,Q11)</f>
         <v>0.44658000000000009</v>
       </c>
       <c r="H11">
-        <f t="shared" ref="H11:H15" si="7">AVERAGE(J11,L11,N11,P11,R11)</f>
+        <f t="shared" ref="H11:H12" si="7">AVERAGE(J11,L11,N11,P11,R11)</f>
         <v>0.26685999999999999</v>
       </c>
       <c r="I11">
@@ -1252,22 +1234,22 @@
       </c>
     </row>
     <row r="12" spans="1:30">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G12">
@@ -1310,22 +1292,22 @@
       </c>
     </row>
     <row r="13" spans="1:30">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="2">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G13">
@@ -1368,22 +1350,22 @@
       </c>
     </row>
     <row r="14" spans="1:30">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G14">
@@ -1456,22 +1438,22 @@
       </c>
     </row>
     <row r="15" spans="1:30">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="D15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="G15">
@@ -1544,22 +1526,22 @@
       </c>
     </row>
     <row r="16" spans="1:30">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="4">
+      <c r="D16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G16">
@@ -1632,22 +1614,22 @@
       </c>
     </row>
     <row r="17" spans="1:30">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="4">
+      <c r="D17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="2">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G17">
@@ -2242,22 +2224,22 @@
       </c>
     </row>
     <row r="29" spans="1:30">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E29" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F29" s="3" t="s">
+      <c r="D29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G29">
@@ -2298,54 +2280,54 @@
       <c r="R29">
         <v>0.30049999999999999</v>
       </c>
-      <c r="U29" s="5">
+      <c r="U29" s="3">
         <v>0.59419999999999995</v>
       </c>
-      <c r="V29" s="5">
+      <c r="V29" s="3">
         <v>0.31330000000000002</v>
       </c>
-      <c r="W29" s="5">
+      <c r="W29" s="3">
         <v>0.59089999999999998</v>
       </c>
-      <c r="X29" s="5">
+      <c r="X29" s="3">
         <v>0.3115</v>
       </c>
-      <c r="Y29" s="5">
+      <c r="Y29" s="3">
         <v>0.58850000000000002</v>
       </c>
-      <c r="Z29" s="5">
+      <c r="Z29" s="3">
         <v>0.29770000000000002</v>
       </c>
-      <c r="AA29" s="5">
+      <c r="AA29" s="3">
         <v>0.59260000000000002</v>
       </c>
-      <c r="AB29" s="5">
+      <c r="AB29" s="3">
         <v>0.3155</v>
       </c>
-      <c r="AC29" s="5">
+      <c r="AC29" s="3">
         <v>0.58689999999999998</v>
       </c>
-      <c r="AD29" s="5">
+      <c r="AD29" s="3">
         <v>0.31430000000000002</v>
       </c>
     </row>
     <row r="30" spans="1:30">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F30" s="3" t="s">
+      <c r="D30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G30">
@@ -2386,54 +2368,54 @@
       <c r="R30">
         <v>0.2351</v>
       </c>
-      <c r="U30" s="5">
+      <c r="U30" s="3">
         <v>0.55700000000000005</v>
       </c>
-      <c r="V30" s="5">
+      <c r="V30" s="3">
         <v>0.26790000000000003</v>
       </c>
-      <c r="W30" s="5">
+      <c r="W30" s="3">
         <v>0.55279999999999996</v>
       </c>
-      <c r="X30" s="5">
+      <c r="X30" s="3">
         <v>0.2472</v>
       </c>
-      <c r="Y30" s="5">
+      <c r="Y30" s="3">
         <v>0.55030000000000001</v>
       </c>
-      <c r="Z30" s="5">
+      <c r="Z30" s="3">
         <v>0.2419</v>
       </c>
-      <c r="AA30" s="5">
+      <c r="AA30" s="3">
         <v>0.53959999999999997</v>
       </c>
-      <c r="AB30" s="5">
+      <c r="AB30" s="3">
         <v>0.17019999999999999</v>
       </c>
-      <c r="AC30" s="5">
+      <c r="AC30" s="3">
         <v>0.55710000000000004</v>
       </c>
-      <c r="AD30" s="5">
+      <c r="AD30" s="3">
         <v>0.2576</v>
       </c>
     </row>
     <row r="31" spans="1:30">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F31" s="3" t="s">
+      <c r="D31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G31">
@@ -2474,54 +2456,54 @@
       <c r="R31">
         <v>0.19650000000000001</v>
       </c>
-      <c r="U31" s="5">
+      <c r="U31" s="3">
         <v>0.55259999999999998</v>
       </c>
-      <c r="V31" s="5">
+      <c r="V31" s="3">
         <v>0.18920000000000001</v>
       </c>
-      <c r="W31" s="5">
+      <c r="W31" s="3">
         <v>0.54430000000000001</v>
       </c>
-      <c r="X31" s="5">
+      <c r="X31" s="3">
         <v>0.2087</v>
       </c>
-      <c r="Y31" s="5">
+      <c r="Y31" s="3">
         <v>0.54649999999999999</v>
       </c>
-      <c r="Z31" s="5">
+      <c r="Z31" s="3">
         <v>0.184</v>
       </c>
-      <c r="AA31" s="5">
+      <c r="AA31" s="3">
         <v>0.55100000000000005</v>
       </c>
-      <c r="AB31" s="5">
+      <c r="AB31" s="3">
         <v>0.1925</v>
       </c>
-      <c r="AC31" s="5">
+      <c r="AC31" s="3">
         <v>0.54869999999999997</v>
       </c>
-      <c r="AD31" s="5">
+      <c r="AD31" s="3">
         <v>0.14219999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:30">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F32" s="3" t="s">
+      <c r="D32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G32">
@@ -2562,54 +2544,54 @@
       <c r="R32">
         <v>0.2742</v>
       </c>
-      <c r="U32" s="5">
+      <c r="U32" s="3">
         <v>0.6038</v>
       </c>
-      <c r="V32" s="5">
+      <c r="V32" s="3">
         <v>0.2616</v>
       </c>
-      <c r="W32" s="5">
+      <c r="W32" s="3">
         <v>0.60970000000000002</v>
       </c>
-      <c r="X32" s="5">
+      <c r="X32" s="3">
         <v>0.25940000000000002</v>
       </c>
-      <c r="Y32" s="5">
+      <c r="Y32" s="3">
         <v>0.60729999999999995</v>
       </c>
-      <c r="Z32" s="5">
+      <c r="Z32" s="3">
         <v>0.26369999999999999</v>
       </c>
-      <c r="AA32" s="5">
+      <c r="AA32" s="3">
         <v>0.60550000000000004</v>
       </c>
-      <c r="AB32" s="5">
+      <c r="AB32" s="3">
         <v>0.26150000000000001</v>
       </c>
-      <c r="AC32" s="5">
+      <c r="AC32" s="3">
         <v>0.60560000000000003</v>
       </c>
-      <c r="AD32" s="5">
+      <c r="AD32" s="3">
         <v>0.28010000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:30">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F33" s="3" t="s">
+      <c r="D33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G33">
@@ -2650,54 +2632,54 @@
       <c r="R33">
         <v>0.14940000000000001</v>
       </c>
-      <c r="U33" s="5">
+      <c r="U33" s="3">
         <v>0.54620000000000002</v>
       </c>
-      <c r="V33" s="5">
+      <c r="V33" s="3">
         <v>0.1535</v>
       </c>
-      <c r="W33" s="5">
+      <c r="W33" s="3">
         <v>0.54269999999999996</v>
       </c>
-      <c r="X33" s="5">
+      <c r="X33" s="3">
         <v>0.2394</v>
       </c>
-      <c r="Y33" s="5">
+      <c r="Y33" s="3">
         <v>0.55159999999999998</v>
       </c>
-      <c r="Z33" s="5">
+      <c r="Z33" s="3">
         <v>0.20250000000000001</v>
       </c>
-      <c r="AA33" s="5">
+      <c r="AA33" s="3">
         <v>0.54630000000000001</v>
       </c>
-      <c r="AB33" s="5">
+      <c r="AB33" s="3">
         <v>0.1535</v>
       </c>
-      <c r="AC33" s="5">
+      <c r="AC33" s="3">
         <v>0.54090000000000005</v>
       </c>
-      <c r="AD33" s="5">
+      <c r="AD33" s="3">
         <v>0.19009999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:30">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F34" s="3" t="s">
+      <c r="D34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G34">
@@ -2738,34 +2720,34 @@
       <c r="R34">
         <v>0.19900000000000001</v>
       </c>
-      <c r="U34" s="5">
+      <c r="U34" s="3">
         <v>0.54669999999999996</v>
       </c>
-      <c r="V34" s="5">
+      <c r="V34" s="3">
         <v>0.16</v>
       </c>
-      <c r="W34" s="5">
+      <c r="W34" s="3">
         <v>0.54900000000000004</v>
       </c>
-      <c r="X34" s="5">
+      <c r="X34" s="3">
         <v>0.21340000000000001</v>
       </c>
-      <c r="Y34" s="5">
+      <c r="Y34" s="3">
         <v>0.55079999999999996</v>
       </c>
-      <c r="Z34" s="5">
+      <c r="Z34" s="3">
         <v>0.1797</v>
       </c>
-      <c r="AA34" s="5">
+      <c r="AA34" s="3">
         <v>0.54769999999999996</v>
       </c>
-      <c r="AB34" s="5">
+      <c r="AB34" s="3">
         <v>0.1673</v>
       </c>
-      <c r="AC34" s="5">
+      <c r="AC34" s="3">
         <v>0.54</v>
       </c>
-      <c r="AD34" s="5">
+      <c r="AD34" s="3">
         <v>0.15909999999999999</v>
       </c>
     </row>
@@ -2789,7 +2771,7 @@
         <v>23</v>
       </c>
       <c r="G35">
-        <f t="shared" ref="G35:G47" si="18">AVERAGE(I35,K35,M35,O35,Q35)</f>
+        <f t="shared" ref="G35:G49" si="18">AVERAGE(I35,K35,M35,O35,Q35)</f>
         <v>0.58864000000000005</v>
       </c>
       <c r="H35">
@@ -2885,7 +2867,7 @@
         <v>0.23139999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:30" ht="16.5" customHeight="1">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -3020,13 +3002,43 @@
       <c r="F39" t="s">
         <v>29</v>
       </c>
-      <c r="G39" t="e">
+      <c r="G39">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H39" t="e">
+        <v>0.63756000000000002</v>
+      </c>
+      <c r="H39">
         <f t="shared" ref="H39" si="20">AVERAGE(J39,L39,N39,O39,R39)</f>
-        <v>#DIV/0!</v>
+        <v>0.30768000000000006</v>
+      </c>
+      <c r="I39">
+        <v>0.64390000000000003</v>
+      </c>
+      <c r="J39">
+        <v>0.23280000000000001</v>
+      </c>
+      <c r="K39">
+        <v>0.63439999999999996</v>
+      </c>
+      <c r="L39">
+        <v>0.23</v>
+      </c>
+      <c r="M39">
+        <v>0.63649999999999995</v>
+      </c>
+      <c r="N39">
+        <v>0.22439999999999999</v>
+      </c>
+      <c r="O39">
+        <v>0.63419999999999999</v>
+      </c>
+      <c r="P39">
+        <v>0.2195</v>
+      </c>
+      <c r="Q39">
+        <v>0.63880000000000003</v>
+      </c>
+      <c r="R39">
+        <v>0.217</v>
       </c>
     </row>
     <row r="40" spans="1:30">
@@ -3048,13 +3060,43 @@
       <c r="F40" t="s">
         <v>30</v>
       </c>
-      <c r="G40" t="e">
+      <c r="G40">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H40" t="e">
+        <v>0.63946000000000003</v>
+      </c>
+      <c r="H40">
         <f t="shared" ref="H40" si="21">AVERAGE(J40,L40,N40,P40,R40)</f>
-        <v>#DIV/0!</v>
+        <v>0.23174</v>
+      </c>
+      <c r="I40">
+        <v>0.63990000000000002</v>
+      </c>
+      <c r="J40">
+        <v>0.2399</v>
+      </c>
+      <c r="K40">
+        <v>0.63790000000000002</v>
+      </c>
+      <c r="L40">
+        <v>0.2409</v>
+      </c>
+      <c r="M40">
+        <v>0.63770000000000004</v>
+      </c>
+      <c r="N40">
+        <v>0.2278</v>
+      </c>
+      <c r="O40">
+        <v>0.64159999999999995</v>
+      </c>
+      <c r="P40">
+        <v>0.2412</v>
+      </c>
+      <c r="Q40">
+        <v>0.64019999999999999</v>
+      </c>
+      <c r="R40">
+        <v>0.2089</v>
       </c>
     </row>
     <row r="42" spans="1:30">
@@ -3065,16 +3107,16 @@
         <v>34</v>
       </c>
       <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42">
+        <v>1E-3</v>
+      </c>
+      <c r="F42" t="s">
         <v>35</v>
-      </c>
-      <c r="D42" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42">
-        <v>1E-3</v>
-      </c>
-      <c r="F42" t="s">
-        <v>36</v>
       </c>
       <c r="G42">
         <f>AVERAGE(I42,K42,M42,O42,Q42)</f>
@@ -3114,30 +3156,30 @@
       <c r="R42">
         <v>0.31359999999999999</v>
       </c>
-      <c r="U42" s="5">
+      <c r="U42" s="3">
         <v>0.56730000000000003</v>
       </c>
-      <c r="V42" s="5">
+      <c r="V42" s="3">
         <v>0.34310000000000002</v>
       </c>
-      <c r="W42" s="5">
+      <c r="W42" s="3">
         <v>0.5645</v>
       </c>
-      <c r="X42" s="5">
+      <c r="X42" s="3">
         <v>0.31590000000000001</v>
       </c>
-      <c r="Y42" s="5"/>
-      <c r="Z42" s="5"/>
-      <c r="AA42" s="5">
+      <c r="Y42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AA42" s="3">
         <v>0.57220000000000004</v>
       </c>
-      <c r="AB42" s="5">
+      <c r="AB42" s="3">
         <v>0.33950000000000002</v>
       </c>
-      <c r="AC42" s="5">
+      <c r="AC42" s="3">
         <v>0.56579999999999997</v>
       </c>
-      <c r="AD42" s="5">
+      <c r="AD42" s="3">
         <v>0.31830000000000003</v>
       </c>
     </row>
@@ -3149,7 +3191,7 @@
         <v>34</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D43" t="s">
         <v>27</v>
@@ -3158,7 +3200,7 @@
         <v>1E-3</v>
       </c>
       <c r="F43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G43">
         <f t="shared" ref="G43:G45" si="23">AVERAGE(I43,K43,M43,O43,Q43)</f>
@@ -3198,34 +3240,34 @@
       <c r="R43">
         <v>0.185</v>
       </c>
-      <c r="U43" s="5">
+      <c r="U43" s="3">
         <v>0.56069999999999998</v>
       </c>
-      <c r="V43" s="5">
+      <c r="V43" s="3">
         <v>0.17710000000000001</v>
       </c>
-      <c r="W43" s="5">
+      <c r="W43" s="3">
         <v>0.56589999999999996</v>
       </c>
-      <c r="X43" s="5">
+      <c r="X43" s="3">
         <v>0.2432</v>
       </c>
-      <c r="Y43" s="5">
+      <c r="Y43" s="3">
         <v>0.5605</v>
       </c>
-      <c r="Z43" s="5">
+      <c r="Z43" s="3">
         <v>0.25059999999999999</v>
       </c>
-      <c r="AA43" s="5">
+      <c r="AA43" s="3">
         <v>0.55179999999999996</v>
       </c>
-      <c r="AB43" s="5">
+      <c r="AB43" s="3">
         <v>0.18210000000000001</v>
       </c>
-      <c r="AC43" s="5">
+      <c r="AC43" s="3">
         <v>0.55779999999999996</v>
       </c>
-      <c r="AD43" s="5">
+      <c r="AD43" s="3">
         <v>0.17399999999999999</v>
       </c>
     </row>
@@ -3237,7 +3279,7 @@
         <v>33</v>
       </c>
       <c r="C44" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D44" t="s">
         <v>27</v>
@@ -3246,7 +3288,7 @@
         <v>1E-3</v>
       </c>
       <c r="F44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G44">
         <f t="shared" si="23"/>
@@ -3286,34 +3328,34 @@
       <c r="R44">
         <v>0.18540000000000001</v>
       </c>
-      <c r="U44" s="5">
+      <c r="U44" s="3">
         <v>0.54690000000000005</v>
       </c>
-      <c r="V44" s="5">
+      <c r="V44" s="3">
         <v>0.17019999999999999</v>
       </c>
-      <c r="W44" s="5">
+      <c r="W44" s="3">
         <v>0.5534</v>
       </c>
-      <c r="X44" s="5">
+      <c r="X44" s="3">
         <v>0.1699</v>
       </c>
-      <c r="Y44" s="5">
+      <c r="Y44" s="3">
         <v>0.5403</v>
       </c>
-      <c r="Z44" s="5">
+      <c r="Z44" s="3">
         <v>0.185</v>
       </c>
-      <c r="AA44" s="5">
+      <c r="AA44" s="3">
         <v>0.54669999999999996</v>
       </c>
-      <c r="AB44" s="5">
+      <c r="AB44" s="3">
         <v>0.1653</v>
       </c>
-      <c r="AC44" s="5">
+      <c r="AC44" s="3">
         <v>0.54090000000000005</v>
       </c>
-      <c r="AD44" s="5">
+      <c r="AD44" s="3">
         <v>0.1757</v>
       </c>
     </row>
@@ -3325,7 +3367,7 @@
         <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D45" t="s">
         <v>27</v>
@@ -3334,7 +3376,7 @@
         <v>1E-3</v>
       </c>
       <c r="F45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G45">
         <f t="shared" si="23"/>
@@ -3374,34 +3416,34 @@
       <c r="R45">
         <v>0.25490000000000002</v>
       </c>
-      <c r="U45" s="5">
+      <c r="U45" s="3">
         <v>0.62429999999999997</v>
       </c>
-      <c r="V45" s="5">
+      <c r="V45" s="3">
         <v>0.27410000000000001</v>
       </c>
-      <c r="W45" s="5">
+      <c r="W45" s="3">
         <v>0.61819999999999997</v>
       </c>
-      <c r="X45" s="5">
+      <c r="X45" s="3">
         <v>0.28320000000000001</v>
       </c>
-      <c r="Y45" s="5"/>
-      <c r="Z45" s="5"/>
-      <c r="AA45" s="5"/>
-      <c r="AB45" s="5"/>
-      <c r="AC45" s="5"/>
-      <c r="AD45" s="5"/>
+      <c r="Y45" s="3"/>
+      <c r="Z45" s="3"/>
+      <c r="AA45" s="3"/>
+      <c r="AB45" s="3"/>
+      <c r="AC45" s="3"/>
+      <c r="AD45" s="3"/>
     </row>
     <row r="46" spans="1:30">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>27</v>
@@ -3410,7 +3452,7 @@
         <v>1E-3</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G46">
         <f t="shared" si="18"/>
@@ -3452,14 +3494,14 @@
       </c>
     </row>
     <row r="47" spans="1:30">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>27</v>
@@ -3468,7 +3510,7 @@
         <v>1E-3</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G47">
         <f t="shared" si="18"/>
@@ -3517,7 +3559,7 @@
         <v>34</v>
       </c>
       <c r="C48" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
@@ -3526,7 +3568,7 @@
         <v>1E-3</v>
       </c>
       <c r="F48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G48">
         <f>AVERAGE(I48,K48,M49,O48,Q48)</f>
@@ -3575,7 +3617,7 @@
         <v>34</v>
       </c>
       <c r="C49" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
         <v>27</v>
@@ -3584,11 +3626,11 @@
         <v>1E-3</v>
       </c>
       <c r="F49" t="s">
-        <v>37</v>
-      </c>
-      <c r="G49" t="e">
-        <f>AVERAGE(I49,K49,#REF!,O49,Q49)</f>
-        <v>#REF!</v>
+        <v>36</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="18"/>
+        <v>0.65564</v>
       </c>
       <c r="H49">
         <f t="shared" si="25"/>
@@ -3633,7 +3675,7 @@
         <v>33</v>
       </c>
       <c r="C50" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D50" t="s">
         <v>27</v>
@@ -3642,7 +3684,7 @@
         <v>1E-3</v>
       </c>
       <c r="F50" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G50">
         <f t="shared" si="25"/>
@@ -3691,7 +3733,7 @@
         <v>33</v>
       </c>
       <c r="C51" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D51" t="s">
         <v>27</v>
@@ -3700,15 +3742,15 @@
         <v>1E-3</v>
       </c>
       <c r="F51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G51">
         <f>AVERAGE(I51,K51,M51,O51,Q51)</f>
-        <v>0.64739999999999998</v>
+        <v>0.65264</v>
       </c>
       <c r="H51">
         <f>AVERAGE(J51,L51,N51,O51,R51)</f>
-        <v>0.24360000000000001</v>
+        <v>0.33106000000000002</v>
       </c>
       <c r="I51">
         <v>0.64739999999999998</v>
@@ -3716,16 +3758,40 @@
       <c r="J51">
         <v>0.24360000000000001</v>
       </c>
+      <c r="K51">
+        <v>0.6573</v>
+      </c>
+      <c r="L51">
+        <v>0.2596</v>
+      </c>
+      <c r="M51">
+        <v>0.65149999999999997</v>
+      </c>
+      <c r="N51">
+        <v>0.2445</v>
+      </c>
+      <c r="O51">
+        <v>0.65269999999999995</v>
+      </c>
+      <c r="P51">
+        <v>0.26069999999999999</v>
+      </c>
+      <c r="Q51">
+        <v>0.65429999999999999</v>
+      </c>
+      <c r="R51">
+        <v>0.25490000000000002</v>
+      </c>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>27</v>
@@ -3734,15 +3800,45 @@
         <v>1E-3</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G52" t="e">
+        <v>39</v>
+      </c>
+      <c r="G52">
         <f>AVERAGE(I52,K52,M52,O52,Q52)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H52" t="e">
+        <v>0.64682000000000006</v>
+      </c>
+      <c r="H52">
         <f>AVERAGE(J52,L52,N52,P52,R52)</f>
-        <v>#DIV/0!</v>
+        <v>0.22023999999999999</v>
+      </c>
+      <c r="I52">
+        <v>0.64670000000000005</v>
+      </c>
+      <c r="J52">
+        <v>0.23630000000000001</v>
+      </c>
+      <c r="K52">
+        <v>0.64319999999999999</v>
+      </c>
+      <c r="L52">
+        <v>0.2198</v>
+      </c>
+      <c r="M52">
+        <v>0.6472</v>
+      </c>
+      <c r="N52">
+        <v>0.2152</v>
+      </c>
+      <c r="O52">
+        <v>0.64890000000000003</v>
+      </c>
+      <c r="P52">
+        <v>0.21829999999999999</v>
+      </c>
+      <c r="Q52">
+        <v>0.64810000000000001</v>
+      </c>
+      <c r="R52">
+        <v>0.21160000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:18">
@@ -3753,7 +3849,7 @@
         <v>33</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>27</v>
@@ -3762,15 +3858,45 @@
         <v>1E-3</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G53" t="e">
+        <v>40</v>
+      </c>
+      <c r="G53">
         <f>AVERAGE(I53,K53,M53,O53,Q53)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H53" t="e">
+        <v>0.64783999999999997</v>
+      </c>
+      <c r="H53">
         <f>AVERAGE(J53,L53,N53,P53,R53)</f>
-        <v>#DIV/0!</v>
+        <v>0.21973999999999999</v>
+      </c>
+      <c r="I53">
+        <v>0.64759999999999995</v>
+      </c>
+      <c r="J53">
+        <v>0.22270000000000001</v>
+      </c>
+      <c r="K53">
+        <v>0.6472</v>
+      </c>
+      <c r="L53">
+        <v>0.2243</v>
+      </c>
+      <c r="M53">
+        <v>0.64690000000000003</v>
+      </c>
+      <c r="N53">
+        <v>0.21909999999999999</v>
+      </c>
+      <c r="O53">
+        <v>0.64770000000000005</v>
+      </c>
+      <c r="P53">
+        <v>0.20660000000000001</v>
+      </c>
+      <c r="Q53">
+        <v>0.64980000000000004</v>
+      </c>
+      <c r="R53">
+        <v>0.22600000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>